<commit_message>
Add comments and remove redundant constraints
</commit_message>
<xml_diff>
--- a/TOP/Bangalore.xlsx
+++ b/TOP/Bangalore.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="395" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="395" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Bannerghatta National Park</t>
-  </si>
-  <si>
-    <t>St. Mary's Basilica</t>
   </si>
   <si>
     <t>HAL Museum</t>
@@ -78,50 +75,35 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="000563C1"/>
-      <sz val="11"/>
-      <u val="single"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,7 +115,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -141,112 +123,49 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  </cellStyleXfs>
+  <cellXfs count="2">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="20">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="15"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000563C1"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -255,17 +174,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C13" activeCellId="0" pane="topLeft" sqref="C13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6377551020408"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -291,7 +212,7 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
@@ -317,7 +238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="13.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
@@ -346,7 +267,7 @@
         <v>360</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="13.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -375,7 +296,7 @@
         <v>120</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>11</v>
       </c>
@@ -404,7 +325,7 @@
         <v>120</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="13.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>12</v>
       </c>
@@ -433,7 +354,7 @@
         <v>120</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="13.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -462,7 +383,7 @@
         <v>180</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
@@ -491,122 +412,94 @@
         <v>210</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="9">
-      <c r="A9" s="2" t="s">
+    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>12.98419</v>
+      <c r="B9" s="0" t="n">
+        <v>12.955272</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>77.6046</v>
+        <v>77.680981</v>
       </c>
       <c r="D9" s="0" t="n">
-        <f aca="false">85*H9/100</f>
-        <v>51</v>
+        <f aca="false">95*H9/100+0.5</f>
+        <v>143</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0</v>
+        <f aca="false">9*60</f>
+        <v>540</v>
       </c>
       <c r="G9" s="0" t="n">
-        <f aca="false">24*60-60</f>
-        <v>1380</v>
+        <f aca="false">17*60-H9</f>
+        <v>870</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>12.955272</v>
+        <v>13.368979</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>77.680981</v>
+        <v>77.683978</v>
       </c>
       <c r="D10" s="0" t="n">
-        <f aca="false">95*H10/100+0.5</f>
-        <v>143</v>
+        <f aca="false">H10*85/100</f>
+        <v>153</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F10" s="0" t="n">
-        <f aca="false">9*60</f>
-        <v>540</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <f aca="false">17*60-H10</f>
-        <v>870</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
-      <c r="A11" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>13.368979</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>77.683978</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <f aca="false">H11*85/100</f>
-        <v>153</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="F11" s="0" t="n">
         <f aca="false">6*60</f>
         <v>360</v>
       </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">18*60-H10</f>
+        <v>900</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>12.974</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>77.714544</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="G11" s="0" t="n">
-        <f aca="false">18*60-H11</f>
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="A12" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>12.974</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>77.714544</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="0" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -621,17 +514,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6377551020408"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -646,17 +540,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6377551020408"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>